<commit_message>
Use pathlib.Path to construct path to benchmarks
Also update xlsx processed files.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/processed/OECM 20220504/benchmark_OECM_PC.xlsx
+++ b/data/processed/OECM 20220504/benchmark_OECM_PC.xlsx
@@ -8533,29 +8533,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A59:A61"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A65:A67"/>
     <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
     <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -31283,167 +31283,167 @@
     </row>
   </sheetData>
   <mergeCells count="161">
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C194:C196"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="A101:A109"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="C179:C181"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="A200:A208"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="C107:C109"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C206:C208"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B176:B178"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B191:B193"/>
+    <mergeCell ref="B107:B109"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="A164:A172"/>
+    <mergeCell ref="B164:B166"/>
     <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B197:B199"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="B206:B208"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C170:C172"/>
+    <mergeCell ref="B203:B205"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="B140:B142"/>
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="A65:A73"/>
-    <mergeCell ref="A74:A82"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A100"/>
-    <mergeCell ref="A101:A109"/>
-    <mergeCell ref="A110:A118"/>
-    <mergeCell ref="A119:A127"/>
-    <mergeCell ref="A128:A136"/>
+    <mergeCell ref="A182:A190"/>
+    <mergeCell ref="B182:B184"/>
+    <mergeCell ref="C137:C139"/>
+    <mergeCell ref="A191:A199"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C197:C199"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C173:C175"/>
+    <mergeCell ref="C188:C190"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C182:C184"/>
+    <mergeCell ref="C71:C73"/>
     <mergeCell ref="A137:A145"/>
     <mergeCell ref="A146:A154"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="A65:A73"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="B158:B160"/>
+    <mergeCell ref="A74:A82"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C158:C160"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B185:B187"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="B50:B52"/>
     <mergeCell ref="A155:A163"/>
-    <mergeCell ref="A164:A172"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C185:C187"/>
+    <mergeCell ref="C200:C202"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="C176:C178"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="B179:B181"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="A110:A118"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C164:C166"/>
+    <mergeCell ref="A119:A127"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="A128:A136"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="C203:C205"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C140:C142"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C191:C193"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="B200:B202"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B170:B172"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="C47:C49"/>
     <mergeCell ref="A173:A181"/>
-    <mergeCell ref="A182:A190"/>
-    <mergeCell ref="A191:A199"/>
-    <mergeCell ref="A200:A208"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="B107:B109"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="C80:C82"/>
     <mergeCell ref="B137:B139"/>
-    <mergeCell ref="B140:B142"/>
-    <mergeCell ref="B143:B145"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="B152:B154"/>
-    <mergeCell ref="B155:B157"/>
-    <mergeCell ref="B158:B160"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="B167:B169"/>
-    <mergeCell ref="B170:B172"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="B176:B178"/>
-    <mergeCell ref="B179:B181"/>
-    <mergeCell ref="B182:B184"/>
-    <mergeCell ref="B185:B187"/>
-    <mergeCell ref="B188:B190"/>
-    <mergeCell ref="B191:B193"/>
-    <mergeCell ref="B194:B196"/>
-    <mergeCell ref="B197:B199"/>
-    <mergeCell ref="B200:B202"/>
-    <mergeCell ref="B203:B205"/>
-    <mergeCell ref="B206:B208"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="C107:C109"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="C119:C121"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="C128:C130"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="C134:C136"/>
-    <mergeCell ref="C137:C139"/>
-    <mergeCell ref="C140:C142"/>
-    <mergeCell ref="C143:C145"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="C152:C154"/>
-    <mergeCell ref="C155:C157"/>
-    <mergeCell ref="C158:C160"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="C164:C166"/>
-    <mergeCell ref="C167:C169"/>
-    <mergeCell ref="C170:C172"/>
-    <mergeCell ref="C173:C175"/>
-    <mergeCell ref="C176:C178"/>
-    <mergeCell ref="C179:C181"/>
-    <mergeCell ref="C182:C184"/>
-    <mergeCell ref="C185:C187"/>
-    <mergeCell ref="C188:C190"/>
-    <mergeCell ref="C191:C193"/>
-    <mergeCell ref="C194:C196"/>
-    <mergeCell ref="C197:C199"/>
-    <mergeCell ref="C200:C202"/>
-    <mergeCell ref="C203:C205"/>
-    <mergeCell ref="C206:C208"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix data error reported in https://github.com/os-climate/itr-data-pipeline/issues/58 Also clean up some import declarations to make pre-commit happier.
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/processed/OECM 20220504/benchmark_OECM_PC.xlsx
+++ b/data/processed/OECM 20220504/benchmark_OECM_PC.xlsx
@@ -21219,34 +21219,34 @@
         <v>3.432480659894455</v>
       </c>
       <c r="AA116" t="n">
-        <v>3.081165145362982</v>
+        <v>3.557173674978253</v>
       </c>
       <c r="AB116" t="n">
-        <v>2.621960522852537</v>
+        <v>3.686396460088829</v>
       </c>
       <c r="AC116" t="n">
-        <v>2.036460284006496</v>
+        <v>3.820313569884533</v>
       </c>
       <c r="AD116" t="n">
-        <v>1.303620116517541</v>
+        <v>3.959095536862635</v>
       </c>
       <c r="AE116" t="n">
-        <v>0.3994107443628224</v>
+        <v>4.102919088518535</v>
       </c>
       <c r="AF116" t="n">
-        <v>0.6559958798575999</v>
+        <v>4.22901941529667</v>
       </c>
       <c r="AG116" t="n">
-        <v>1.077413666166268</v>
+        <v>4.358995346752959</v>
       </c>
       <c r="AH116" t="n">
-        <v>1.769554114110935</v>
+        <v>4.492965996865972</v>
       </c>
       <c r="AI116" t="n">
-        <v>2.906331951319155</v>
+        <v>4.631054140498466</v>
       </c>
       <c r="AJ116" t="n">
-        <v>4.773386325912086</v>
+        <v>4.773386325912084</v>
       </c>
     </row>
     <row r="117">
@@ -21325,34 +21325,34 @@
         <v>3.451582319375555</v>
       </c>
       <c r="AA117" t="n">
-        <v>3.100597750146336</v>
+        <v>3.576322073469606</v>
       </c>
       <c r="AB117" t="n">
-        <v>2.641591676446237</v>
+        <v>3.705569906702924</v>
       </c>
       <c r="AC117" t="n">
-        <v>2.056127017321181</v>
+        <v>3.839488740492773</v>
       </c>
       <c r="AD117" t="n">
-        <v>1.32312401614709</v>
+        <v>3.978247384216093</v>
       </c>
       <c r="AE117" t="n">
-        <v>0.4185124038439192</v>
+        <v>4.122020747999633</v>
       </c>
       <c r="AF117" t="n">
-        <v>0.6815204215206923</v>
+        <v>4.248154912953026</v>
       </c>
       <c r="AG117" t="n">
-        <v>1.10981199286739</v>
+        <v>4.378148793453997</v>
       </c>
       <c r="AH117" t="n">
-        <v>1.807257157113512</v>
+        <v>4.512120497107363</v>
       </c>
       <c r="AI117" t="n">
-        <v>2.94300156506624</v>
+        <v>4.650191745620103</v>
       </c>
       <c r="AJ117" t="n">
-        <v>4.79248798539318</v>
+        <v>4.792487985393181</v>
       </c>
     </row>
     <row r="118">
@@ -24165,34 +24165,34 @@
         <v>60.3345961688895</v>
       </c>
       <c r="AA143" t="n">
-        <v>52.77345136866046</v>
+        <v>59.51245099862201</v>
       </c>
       <c r="AB143" t="n">
-        <v>43.86572449779822</v>
+        <v>58.43527029199462</v>
       </c>
       <c r="AC143" t="n">
-        <v>33.51302352318868</v>
+        <v>57.08816830008796</v>
       </c>
       <c r="AD143" t="n">
-        <v>21.61689418744947</v>
+        <v>55.45667720189595</v>
       </c>
       <c r="AE143" t="n">
-        <v>8.079347585262525</v>
+        <v>53.52682953577428</v>
       </c>
       <c r="AF143" t="n">
-        <v>11.4104233484326</v>
+        <v>53.94142129762501</v>
       </c>
       <c r="AG143" t="n">
-        <v>16.50902315756966</v>
+        <v>54.36843509717605</v>
       </c>
       <c r="AH143" t="n">
-        <v>24.38637574544474</v>
+        <v>54.8144568700821</v>
       </c>
       <c r="AI143" t="n">
-        <v>36.64017081978882</v>
+        <v>55.28691731479681</v>
       </c>
       <c r="AJ143" t="n">
-        <v>55.79415771690534</v>
+        <v>55.79415771690532</v>
       </c>
     </row>
     <row r="144">
@@ -24271,31 +24271,31 @@
         <v>61.06917477899204</v>
       </c>
       <c r="AA144" t="n">
-        <v>53.523224273176</v>
+        <v>60.25820030696759</v>
       </c>
       <c r="AB144" t="n">
-        <v>44.62840843286062</v>
+        <v>59.19168932884531</v>
       </c>
       <c r="AC144" t="n">
-        <v>34.2860445309702</v>
+        <v>57.85469288685603</v>
       </c>
       <c r="AD144" t="n">
-        <v>22.39738206169243</v>
+        <v>56.23267873348955</v>
       </c>
       <c r="AE144" t="n">
-        <v>8.864132139490557</v>
+        <v>54.31161409000232</v>
       </c>
       <c r="AF144" t="n">
-        <v>12.28836134449532</v>
+        <v>54.74330818043516</v>
       </c>
       <c r="AG144" t="n">
-        <v>17.47736052459711</v>
+        <v>55.1839670743574</v>
       </c>
       <c r="AH144" t="n">
-        <v>25.41822494037765</v>
+        <v>55.63906728212835</v>
       </c>
       <c r="AI144" t="n">
-        <v>37.657526860132</v>
+        <v>56.11472693285933</v>
       </c>
       <c r="AJ144" t="n">
         <v>56.61774280794361</v>

</xml_diff>